<commit_message>
+Add dynamic keyboard change between English/Number, user/password check.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35643" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37865" uniqueCount="328">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1378,6 +1378,24 @@
 The demo will save the unlock log on the internal flash rom and restore when next time power reset.
 When you input correct user and password, the VCOM will send the unlock package and unlock log will add 1 record.
 Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000-00-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-00-00 00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InputData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hack-Regular.ttf</t>
   </si>
 </sst>
 </file>
@@ -3086,7 +3104,7 @@
         <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="F17" t="s">
         <v>67</v>
@@ -3483,7 +3501,23 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="4:4"/>
+    <row r="41" spans="4:4">
+      <c r="B41" t="s">
+        <v>322</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" t="s">
+        <v>325</v>
+      </c>
+      <c r="F41" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="42" spans="4:4"/>
     <row r="43" spans="4:4"/>
     <row r="44" spans="4:4"/>

</xml_diff>

<commit_message>
+Add show 1 log.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44346" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45882" uniqueCount="352">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1454,6 +1454,21 @@
   </si>
   <si>
     <t xml:space="preserve">2018-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9999-99-99 99:99:99&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -3081,7 +3096,7 @@
         <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F11" t="s">
         <v>67</v>
@@ -3098,7 +3113,7 @@
         <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F12" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
+Add read log list.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45882" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47165" uniqueCount="353">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1469,6 +1469,9 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9,0x0020-0x0060</t>
   </si>
 </sst>
 </file>
@@ -2709,7 +2712,7 @@
         <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="I4"/>
       <c r="K4" s="12" t="s">
@@ -2779,8 +2782,12 @@
         <v>4</v>
       </c>
       <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>352</v>
+      </c>
       <c r="I6"/>
       <c r="K6" s="15" t="s">
         <v>2</v>
@@ -3249,7 +3256,7 @@
         <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F20" t="s">
         <v>67</v>
@@ -3266,7 +3273,7 @@
         <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F21" t="s">
         <v>67</v>
@@ -3300,7 +3307,7 @@
         <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F23" t="s">
         <v>67</v>
@@ -3317,7 +3324,7 @@
         <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F24" t="s">
         <v>67</v>
@@ -3351,7 +3358,7 @@
         <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F26" t="s">
         <v>67</v>
@@ -3368,7 +3375,7 @@
         <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F27" t="s">
         <v>67</v>
@@ -3402,7 +3409,7 @@
         <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F29" t="s">
         <v>67</v>
@@ -3419,7 +3426,7 @@
         <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F30" t="s">
         <v>67</v>
@@ -3453,7 +3460,7 @@
         <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F32" t="s">
         <v>67</v>
@@ -3470,7 +3477,7 @@
         <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F33" t="s">
         <v>67</v>
@@ -3504,7 +3511,7 @@
         <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F35" t="s">
         <v>67</v>
@@ -3521,7 +3528,7 @@
         <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F36" t="s">
         <v>67</v>
@@ -3555,7 +3562,7 @@
         <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="F38" t="s">
         <v>67</v>
@@ -3572,7 +3579,7 @@
         <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="F39" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
+Update English keyboard key.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47165" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47939" uniqueCount="354">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1472,6 +1472,9 @@
   </si>
   <si>
     <t xml:space="preserve">a-z,A-Z,0-9,0x0020-0x0060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Medium.ttf</t>
   </si>
 </sst>
 </file>
@@ -2697,10 +2700,10 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>353</v>
       </c>
       <c r="D4">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -2736,7 +2739,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>353</v>
       </c>
       <c r="D5">
         <v>40</v>

</xml_diff>

<commit_message>
+Info, Config screen done.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48962" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56145" uniqueCount="380">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1484,6 +1484,153 @@
   </si>
   <si>
     <t xml:space="preserve">KohinoorBangla.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will continue to be innovative and perform extensive efforts to bring highly reliable products to the market. The products we make will have optimal viewing performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+The products we make will have optimal viewing performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+The products we make will have optimal viewing performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+The products we make will have optimal viewing performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+The products we make will have optimal viewing performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+The products we make will have optimal viewing performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDT is a leader within the embedded market. We will 
+continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+The products we make will have optimal viewing 
+performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  EDT is a leader within the embedded market. We will 
+continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+  The products we make will have optimal viewing 
+performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    EDT is a leader within the embedded market. We will 
+continue to be innovative and perform extensive efforts to bring highly reliable products to the market. 
+    The products we make will have optimal viewing 
+performance, as well as being user friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Security Box Demo is for show you the concept that 
+Smart Embedded can do.
+The demo will save the unlock log on the internal flash 
+rom and restore when next time power reset.
+When you input correct user and password, the VCOM will send the unlock package and unlock log will add 1 record.
+Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do.
+    The demo will save the unlock log on the internal flash 
+rom and restore when next time power reset.
+    When you input correct user and password, the VCOM will send the unlock package and unlock log will add 1 record.
+Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock log on the internal flash rom and restore when next time power reset.
+Input correct user and password, the VCOM will send the unlock package and unlock log will add 1 
+record.
+Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock log on the internal flash rom and restore when next time power reset.
+Input correct user and password, the VCOM will send the unlock package and unlock log will add 1 
+record.
+Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time power reset.
+Input correct user and password, the VCOM will send the 
+unlock package and unlock log will add 1 
+record.
+Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time power reset.
+    Input correct user and password, the VCOM will send the 
+unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time power reset.
+    Input correct user and password, the VCOM will send the 
+unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the VCOM will send 
+the unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the VCOM will send 
+the unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the VCOM will send 
+the unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the VCOM will send 
+the unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the VCOM will send 
+the unlock package and unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConfigButton</t>
   </si>
 </sst>
 </file>
@@ -2892,6 +3039,28 @@
       <c r="O8" s="18"/>
     </row>
     <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C9" t="s">
+        <v>356</v>
+      </c>
+      <c r="D9">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>352</v>
+      </c>
+      <c r="I9"/>
       <c r="K9" s="19" t="s">
         <v>28</v>
       </c>
@@ -2909,6 +3078,28 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C10" t="s">
+        <v>356</v>
+      </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10"/>
       <c r="K10" s="27" t="s">
         <v>50</v>
       </c>
@@ -3080,7 +3271,7 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>379</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -3131,13 +3322,13 @@
         <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
       <c r="D11" t="s">
         <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>164</v>
+        <v>366</v>
       </c>
       <c r="F11" t="s">
         <v>67</v>
@@ -3148,7 +3339,7 @@
         <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
@@ -3165,7 +3356,7 @@
         <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
       <c r="D13" t="s">
         <v>61</v>
@@ -3199,13 +3390,13 @@
         <v>170</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
       <c r="D15" t="s">
         <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>306</v>
+        <v>375</v>
       </c>
       <c r="F15" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
+Completed UI of log, config screen.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56145" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58521" uniqueCount="382">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1631,6 +1631,12 @@
   </si>
   <si>
     <t xml:space="preserve">ConfigButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogColumn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogRecord</t>
   </si>
 </sst>
 </file>
@@ -2929,13 +2935,13 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -3115,6 +3121,28 @@
       <c r="O10" s="28"/>
     </row>
     <row r="11" spans="2:15">
+      <c r="B11" t="s">
+        <v>380</v>
+      </c>
+      <c r="C11" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>352</v>
+      </c>
+      <c r="I11"/>
       <c r="K11" s="23"/>
       <c r="L11" s="24"/>
     </row>
@@ -3237,7 +3265,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>380</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -3254,7 +3282,7 @@
         <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>380</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -3288,7 +3316,7 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D9" t="s">
         <v>61</v>
@@ -3305,7 +3333,7 @@
         <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D10" t="s">
         <v>61</v>
@@ -3370,16 +3398,16 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
       <c r="D14" t="s">
         <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>375</v>
       </c>
       <c r="F14" t="s">
         <v>67</v>
@@ -3387,16 +3415,16 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>357</v>
+        <v>380</v>
       </c>
       <c r="D15" t="s">
         <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>375</v>
+        <v>181</v>
       </c>
       <c r="F15" t="s">
         <v>67</v>
@@ -3404,16 +3432,16 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>380</v>
       </c>
       <c r="D16" t="s">
         <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F16" t="s">
         <v>67</v>
@@ -3421,16 +3449,16 @@
     </row>
     <row r="17" spans="4:4">
       <c r="B17" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D17" t="s">
         <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>183</v>
+        <v>350</v>
       </c>
       <c r="F17" t="s">
         <v>67</v>
@@ -3438,10 +3466,10 @@
     </row>
     <row r="18" spans="4:4">
       <c r="B18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D18" t="s">
         <v>61</v>
@@ -3455,16 +3483,16 @@
     </row>
     <row r="19" spans="4:4">
       <c r="B19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>380</v>
       </c>
       <c r="D19" t="s">
         <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>350</v>
+        <v>193</v>
       </c>
       <c r="F19" t="s">
         <v>67</v>
@@ -3472,16 +3500,16 @@
     </row>
     <row r="20" spans="4:4">
       <c r="B20" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D20" t="s">
         <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>193</v>
+        <v>350</v>
       </c>
       <c r="F20" t="s">
         <v>67</v>
@@ -3489,10 +3517,10 @@
     </row>
     <row r="21" spans="4:4">
       <c r="B21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D21" t="s">
         <v>61</v>
@@ -3506,16 +3534,16 @@
     </row>
     <row r="22" spans="4:4">
       <c r="B22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D22" t="s">
         <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>350</v>
+        <v>209</v>
       </c>
       <c r="F22" t="s">
         <v>67</v>
@@ -3523,16 +3551,16 @@
     </row>
     <row r="23" spans="4:4">
       <c r="B23" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D23" t="s">
         <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>350</v>
       </c>
       <c r="F23" t="s">
         <v>67</v>
@@ -3540,10 +3568,10 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -3557,16 +3585,16 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D25" t="s">
         <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>350</v>
+        <v>223</v>
       </c>
       <c r="F25" t="s">
         <v>67</v>
@@ -3574,16 +3602,16 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D26" t="s">
         <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>223</v>
+        <v>350</v>
       </c>
       <c r="F26" t="s">
         <v>67</v>
@@ -3591,10 +3619,10 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D27" t="s">
         <v>61</v>
@@ -3608,16 +3636,16 @@
     </row>
     <row r="28" spans="4:4">
       <c r="B28" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D28" t="s">
         <v>61</v>
       </c>
       <c r="E28" t="s">
-        <v>350</v>
+        <v>236</v>
       </c>
       <c r="F28" t="s">
         <v>67</v>
@@ -3625,16 +3653,16 @@
     </row>
     <row r="29" spans="4:4">
       <c r="B29" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D29" t="s">
         <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>236</v>
+        <v>350</v>
       </c>
       <c r="F29" t="s">
         <v>67</v>
@@ -3642,10 +3670,10 @@
     </row>
     <row r="30" spans="4:4">
       <c r="B30" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D30" t="s">
         <v>61</v>
@@ -3659,16 +3687,16 @@
     </row>
     <row r="31" spans="4:4">
       <c r="B31" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D31" t="s">
         <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>350</v>
+        <v>244</v>
       </c>
       <c r="F31" t="s">
         <v>67</v>
@@ -3676,16 +3704,16 @@
     </row>
     <row r="32" spans="4:4">
       <c r="B32" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D32" t="s">
         <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>244</v>
+        <v>350</v>
       </c>
       <c r="F32" t="s">
         <v>67</v>
@@ -3693,10 +3721,10 @@
     </row>
     <row r="33" spans="4:4">
       <c r="B33" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
@@ -3710,16 +3738,16 @@
     </row>
     <row r="34" spans="4:4">
       <c r="B34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="F34" t="s">
         <v>67</v>
@@ -3727,16 +3755,16 @@
     </row>
     <row r="35" spans="4:4">
       <c r="B35" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D35" t="s">
         <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="F35" t="s">
         <v>67</v>
@@ -3744,10 +3772,10 @@
     </row>
     <row r="36" spans="4:4">
       <c r="B36" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D36" t="s">
         <v>61</v>
@@ -3761,16 +3789,16 @@
     </row>
     <row r="37" spans="4:4">
       <c r="B37" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="D37" t="s">
         <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>350</v>
+        <v>254</v>
       </c>
       <c r="F37" t="s">
         <v>67</v>
@@ -3778,16 +3806,16 @@
     </row>
     <row r="38" spans="4:4">
       <c r="B38" t="s">
-        <v>253</v>
+        <v>334</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>334</v>
       </c>
       <c r="D38" t="s">
         <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>254</v>
+        <v>339</v>
       </c>
       <c r="F38" t="s">
         <v>67</v>
@@ -3795,7 +3823,7 @@
     </row>
     <row r="39" spans="4:4">
       <c r="B39" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C39" t="s">
         <v>334</v>
@@ -3804,29 +3832,13 @@
         <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="F39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
-      <c r="B40" t="s">
-        <v>322</v>
-      </c>
-      <c r="C40" t="s">
-        <v>334</v>
-      </c>
-      <c r="D40" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" t="s">
-        <v>346</v>
-      </c>
-      <c r="F40" t="s">
-        <v>67</v>
-      </c>
-    </row>
+    <row r="40" spans="4:4"/>
     <row r="41" spans="4:4"/>
     <row r="42" spans="4:4"/>
     <row r="43" spans="4:4"/>

</xml_diff>

<commit_message>
+Add clear unlock log. +Remove USART feature.
</commit_message>
<xml_diff>
--- a/touchgfx/demo/security-box/assets/texts/texts.xlsx
+++ b/touchgfx/demo/security-box/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58521" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59041" uniqueCount="384">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1637,6 +1637,22 @@
   </si>
   <si>
     <t xml:space="preserve">LogRecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    The Security Box Demo is for show you the concept that 
+Smart Embedded can do. The demo will save the unlock 
+log on the internal flash rom and restore when next time 
+power reset.
+    Input correct user and password, the unlock log will add 1 record.
+    Try username, password : "EDT, 3038" or "ROJAR, 3683".</t>
   </si>
 </sst>
 </file>
@@ -3407,7 +3423,7 @@
         <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="F14" t="s">
         <v>67</v>

</xml_diff>